<commit_message>
updated discussion of coding
</commit_message>
<xml_diff>
--- a/assets/slides/acct3210/S5/E2.xlsx
+++ b/assets/slides/acct3210/S5/E2.xlsx
@@ -1,56 +1,89 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shamussiothrun/ArthurHowardMorris.github.io/assets/slides/acct3210/S5/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ahmlaoibhtighe/ArthurHowardMorris.github.io/assets/slides/acct3210/S5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{124F85C6-5D9B-284F-A0A3-66136D991573}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7FFEF86-3F71-714B-95F9-62E02D2B02DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25640" yWindow="600" windowWidth="25500" windowHeight="42500" activeTab="1" xr2:uid="{2705985C-3817-8A49-B643-240FB205B502}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20940" xr2:uid="{2705985C-3817-8A49-B643-240FB205B502}"/>
   </bookViews>
   <sheets>
-    <sheet name="Answer Report 1" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="E2 blank" sheetId="4" r:id="rId1"/>
+    <sheet name="E2 solution" sheetId="1" r:id="rId2"/>
+    <sheet name="Answer Report E2" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="solver_adj" localSheetId="1" hidden="1">Sheet1!$B$3:$C$3</definedName>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">'E2 blank'!$B$3:$C$3</definedName>
+    <definedName name="solver_adj" localSheetId="1" hidden="1">'E2 solution'!$B$3:$C$3</definedName>
+    <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
-    <definedName name="solver_lhs1" localSheetId="1" hidden="1">Sheet1!$B$10</definedName>
-    <definedName name="solver_lhs2" localSheetId="1" hidden="1">Sheet1!$B$9</definedName>
+    <definedName name="solver_lhs1" localSheetId="0" hidden="1">'E2 blank'!$B$10</definedName>
+    <definedName name="solver_lhs1" localSheetId="1" hidden="1">'E2 solution'!$B$10</definedName>
+    <definedName name="solver_lhs2" localSheetId="0" hidden="1">'E2 blank'!$B$9</definedName>
+    <definedName name="solver_lhs2" localSheetId="1" hidden="1">'E2 solution'!$B$9</definedName>
+    <definedName name="solver_lin" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_lin" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_num" localSheetId="1" hidden="1">2</definedName>
-    <definedName name="solver_opt" localSheetId="1" hidden="1">Sheet1!$B$6</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">'E2 blank'!$B$6</definedName>
+    <definedName name="solver_opt" localSheetId="1" hidden="1">'E2 solution'!$B$6</definedName>
+    <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel2" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel2" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_rhs1" localSheetId="1" hidden="1">Sheet1!$C$10</definedName>
-    <definedName name="solver_rhs2" localSheetId="1" hidden="1">Sheet1!$C$9</definedName>
+    <definedName name="solver_rhs1" localSheetId="0" hidden="1">'E2 blank'!$C$10</definedName>
+    <definedName name="solver_rhs1" localSheetId="1" hidden="1">'E2 solution'!$C$10</definedName>
+    <definedName name="solver_rhs2" localSheetId="0" hidden="1">'E2 blank'!$C$9</definedName>
+    <definedName name="solver_rhs2" localSheetId="1" hidden="1">'E2 solution'!$C$9</definedName>
+    <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="1" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_ver" localSheetId="1" hidden="1">2</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -71,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="46">
   <si>
     <t>Choice variables</t>
   </si>
@@ -303,18 +336,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -357,7 +388,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$12</c:f>
+              <c:f>'E2 blank'!$B$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -380,77 +411,17 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$13:$B$32</c:f>
+              <c:f>'E2 blank'!$B$13:$B$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
-                <c:pt idx="0">
-                  <c:v>7.6</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>7.2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6.8</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6.4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5.6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>5.2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4.8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4.4000000000000004</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>3.6</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>3.2</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2.8</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>2.4</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1.6</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1.2</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.8</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.4</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-4A49-F646-9371-F3096833435E}"/>
+              <c16:uniqueId val="{00000000-4678-714B-9DB8-904E2962C3F8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -459,7 +430,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$12</c:f>
+              <c:f>'E2 blank'!$C$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -482,7 +453,341 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$13:$C$32</c:f>
+              <c:f>'E2 blank'!$C$13:$C$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4678-714B-9DB8-904E2962C3F8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1737674703"/>
+        <c:axId val="1738340271"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1737674703"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1738340271"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1738340271"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1737674703"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'E2 solution'!$B$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>frame const</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'E2 solution'!$B$13:$B$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>7.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4A49-F646-9371-F3096833435E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'E2 solution'!$C$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>roof const</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'E2 solution'!$C$13:$C$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -766,6 +1071,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -1282,7 +1627,566 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>494632</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>112295</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>93579</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>48126</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4808AF37-9A9F-594F-9079-A4F4DB5F3A3B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1324,9 +2228,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1364,7 +2268,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1470,7 +2374,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1612,13 +2516,564 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5104249-C563-C245-80DF-01B43C5C87B7}">
+  <dimension ref="A1:C32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:C32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{431352B3-90D6-6C42-8907-460D7ACBF989}">
+  <dimension ref="A1:C32"/>
+  <sheetViews>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>8.1818181818181834</v>
+      </c>
+      <c r="C3" s="1">
+        <v>4.7272727272727266</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>300</v>
+      </c>
+      <c r="C4">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <f>B3*B4</f>
+        <v>2454.545454545455</v>
+      </c>
+      <c r="C5">
+        <f>C3*C4</f>
+        <v>2694.545454545454</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2">
+        <f>SUM(B5:C5)</f>
+        <v>5149.090909090909</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B9">
+        <f>4*B3+10*C3</f>
+        <v>80</v>
+      </c>
+      <c r="C9">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B10">
+        <f>5*B3+7*C3</f>
+        <v>74</v>
+      </c>
+      <c r="C10">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <f>(80-4*A13)/10</f>
+        <v>7.6</v>
+      </c>
+      <c r="C13">
+        <f>(74-5*A13)/7</f>
+        <v>9.8571428571428577</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <f t="shared" ref="B14:B32" si="0">(80-4*A14)/10</f>
+        <v>7.2</v>
+      </c>
+      <c r="C14">
+        <f t="shared" ref="C14:C32" si="1">(74-5*A14)/7</f>
+        <v>9.1428571428571423</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>3</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>6.8</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="1"/>
+        <v>8.4285714285714288</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>4</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>6.4</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="1"/>
+        <v>7.7142857142857144</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>5</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>6</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>5.6</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="1"/>
+        <v>6.2857142857142856</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>7</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>5.2</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="1"/>
+        <v>5.5714285714285712</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>8</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>4.8</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="1"/>
+        <v>4.8571428571428568</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>9</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="1"/>
+        <v>4.1428571428571432</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>10</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="1"/>
+        <v>3.4285714285714284</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>11</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>3.6</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="1"/>
+        <v>2.7142857142857144</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>12</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="0"/>
+        <v>3.2</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>13</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="0"/>
+        <v>2.8</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="1"/>
+        <v>1.2857142857142858</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>14</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="0"/>
+        <v>2.4</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="1"/>
+        <v>0.5714285714285714</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>15</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="1"/>
+        <v>-0.14285714285714285</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>16</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="0"/>
+        <v>1.6</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="1"/>
+        <v>-0.8571428571428571</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>17</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="1"/>
+        <v>-1.5714285714285714</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>18</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="1"/>
+        <v>-2.2857142857142856</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>19</v>
+      </c>
+      <c r="B31">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="1"/>
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>20</v>
+      </c>
+      <c r="B32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="1"/>
+        <v>-3.7142857142857144</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{587B4097-1C5A-634F-B034-281F763A6B3D}">
   <dimension ref="A1:G28"/>
   <sheetViews>
@@ -1719,10 +3174,10 @@
       <c r="C16" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="4">
         <v>870</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="4">
         <v>5149.090909090909</v>
       </c>
     </row>
@@ -1755,10 +3210,10 @@
       <c r="C21" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D21" s="8">
+      <c r="D21" s="6">
         <v>1</v>
       </c>
-      <c r="E21" s="8">
+      <c r="E21" s="6">
         <v>8.1818181818181834</v>
       </c>
       <c r="F21" s="6" t="s">
@@ -1772,10 +3227,10 @@
       <c r="C22" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D22" s="7">
+      <c r="D22" s="4">
         <v>1</v>
       </c>
-      <c r="E22" s="7">
+      <c r="E22" s="4">
         <v>4.7272727272727266</v>
       </c>
       <c r="F22" s="4" t="s">
@@ -1814,7 +3269,7 @@
       <c r="C27" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D27" s="8">
+      <c r="D27" s="6">
         <v>74</v>
       </c>
       <c r="E27" s="6" t="s">
@@ -1834,7 +3289,7 @@
       <c r="C28" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D28" s="7">
+      <c r="D28" s="4">
         <v>80</v>
       </c>
       <c r="E28" s="4" t="s">
@@ -1850,379 +3305,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{431352B3-90D6-6C42-8907-460D7ACBF989}">
-  <dimension ref="A1:C32"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1">
-        <v>8.1818181818181834</v>
-      </c>
-      <c r="C3" s="1">
-        <v>4.7272727272727266</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>300</v>
-      </c>
-      <c r="C4">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <f>B3*B4</f>
-        <v>2454.545454545455</v>
-      </c>
-      <c r="C5">
-        <f>C3*C4</f>
-        <v>2694.545454545454</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="2">
-        <f>SUM(B5:C5)</f>
-        <v>5149.090909090909</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9">
-        <f>4*B3+10*C3</f>
-        <v>80</v>
-      </c>
-      <c r="C9">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10">
-        <f>5*B3+7*C3</f>
-        <v>74</v>
-      </c>
-      <c r="C10">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>1</v>
-      </c>
-      <c r="B13">
-        <f>(80-4*A13)/10</f>
-        <v>7.6</v>
-      </c>
-      <c r="C13">
-        <f>(74-5*A13)/7</f>
-        <v>9.8571428571428577</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>2</v>
-      </c>
-      <c r="B14">
-        <f t="shared" ref="B14:B32" si="0">(80-4*A14)/10</f>
-        <v>7.2</v>
-      </c>
-      <c r="C14">
-        <f t="shared" ref="C14:C32" si="1">(74-5*A14)/7</f>
-        <v>9.1428571428571423</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>3</v>
-      </c>
-      <c r="B15">
-        <f t="shared" si="0"/>
-        <v>6.8</v>
-      </c>
-      <c r="C15">
-        <f t="shared" si="1"/>
-        <v>8.4285714285714288</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>4</v>
-      </c>
-      <c r="B16">
-        <f t="shared" si="0"/>
-        <v>6.4</v>
-      </c>
-      <c r="C16">
-        <f t="shared" si="1"/>
-        <v>7.7142857142857144</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>5</v>
-      </c>
-      <c r="B17">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="C17">
-        <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>6</v>
-      </c>
-      <c r="B18">
-        <f t="shared" si="0"/>
-        <v>5.6</v>
-      </c>
-      <c r="C18">
-        <f t="shared" si="1"/>
-        <v>6.2857142857142856</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>7</v>
-      </c>
-      <c r="B19">
-        <f t="shared" si="0"/>
-        <v>5.2</v>
-      </c>
-      <c r="C19">
-        <f t="shared" si="1"/>
-        <v>5.5714285714285712</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>8</v>
-      </c>
-      <c r="B20">
-        <f t="shared" si="0"/>
-        <v>4.8</v>
-      </c>
-      <c r="C20">
-        <f t="shared" si="1"/>
-        <v>4.8571428571428568</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>9</v>
-      </c>
-      <c r="B21">
-        <f t="shared" si="0"/>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="C21">
-        <f t="shared" si="1"/>
-        <v>4.1428571428571432</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>10</v>
-      </c>
-      <c r="B22">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="C22">
-        <f t="shared" si="1"/>
-        <v>3.4285714285714284</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>11</v>
-      </c>
-      <c r="B23">
-        <f t="shared" si="0"/>
-        <v>3.6</v>
-      </c>
-      <c r="C23">
-        <f t="shared" si="1"/>
-        <v>2.7142857142857144</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>12</v>
-      </c>
-      <c r="B24">
-        <f t="shared" si="0"/>
-        <v>3.2</v>
-      </c>
-      <c r="C24">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>13</v>
-      </c>
-      <c r="B25">
-        <f t="shared" si="0"/>
-        <v>2.8</v>
-      </c>
-      <c r="C25">
-        <f t="shared" si="1"/>
-        <v>1.2857142857142858</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>14</v>
-      </c>
-      <c r="B26">
-        <f t="shared" si="0"/>
-        <v>2.4</v>
-      </c>
-      <c r="C26">
-        <f t="shared" si="1"/>
-        <v>0.5714285714285714</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>15</v>
-      </c>
-      <c r="B27">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="C27">
-        <f t="shared" si="1"/>
-        <v>-0.14285714285714285</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>16</v>
-      </c>
-      <c r="B28">
-        <f t="shared" si="0"/>
-        <v>1.6</v>
-      </c>
-      <c r="C28">
-        <f t="shared" si="1"/>
-        <v>-0.8571428571428571</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>17</v>
-      </c>
-      <c r="B29">
-        <f t="shared" si="0"/>
-        <v>1.2</v>
-      </c>
-      <c r="C29">
-        <f t="shared" si="1"/>
-        <v>-1.5714285714285714</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>18</v>
-      </c>
-      <c r="B30">
-        <f t="shared" si="0"/>
-        <v>0.8</v>
-      </c>
-      <c r="C30">
-        <f t="shared" si="1"/>
-        <v>-2.2857142857142856</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <v>19</v>
-      </c>
-      <c r="B31">
-        <f t="shared" si="0"/>
-        <v>0.4</v>
-      </c>
-      <c r="C31">
-        <f t="shared" si="1"/>
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <v>20</v>
-      </c>
-      <c r="B32">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C32">
-        <f t="shared" si="1"/>
-        <v>-3.7142857142857144</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>